<commit_message>
cam 1-8 calibration and validation
</commit_message>
<xml_diff>
--- a/Cam3calib.xlsx
+++ b/Cam3calib.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C4409C-CE7E-4B0F-AE62-9CF8EBAF9BFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590D8501-85D2-4E70-9910-DABF349E7936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17923" yWindow="2966" windowWidth="24686" windowHeight="13217" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18043" yWindow="3429" windowWidth="16191" windowHeight="13217" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,20 +345,20 @@
   <dimension ref="A1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
-        <v>860.19600000000003</v>
+        <v>898.53200000000004</v>
       </c>
       <c r="B1" s="1">
-        <v>1022.479</v>
+        <v>1022.3579999999999</v>
       </c>
       <c r="C1" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D1" s="1">
         <v>0</v>
@@ -367,268 +367,268 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>884.99699999999996</v>
+        <v>917.84900000000005</v>
       </c>
       <c r="B2" s="1">
-        <v>1797.22</v>
+        <v>1774.625</v>
       </c>
       <c r="C2" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D2" s="1">
-        <v>-16.07</v>
+        <v>-16.079999999999998</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>879.12199999999996</v>
+        <v>912.96299999999997</v>
       </c>
       <c r="B3" s="1">
-        <v>1691.8530000000001</v>
+        <v>1669.713</v>
       </c>
       <c r="C3" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D3" s="1">
-        <v>-13.98</v>
+        <v>-13.97</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>874.99199999999996</v>
+        <v>908.98599999999999</v>
       </c>
       <c r="B4" s="1">
-        <v>1593.278</v>
+        <v>1572.4860000000001</v>
       </c>
       <c r="C4" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D4" s="1">
-        <v>-11.98</v>
+        <v>-11.95</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>870.59500000000003</v>
+        <v>905.73500000000001</v>
       </c>
       <c r="B5" s="1">
-        <v>1495.8789999999999</v>
+        <v>1476.883</v>
       </c>
       <c r="C5" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D5" s="1">
-        <v>-9.98</v>
+        <v>-9.9499999999999993</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>867.53200000000004</v>
+        <v>902.96299999999997</v>
       </c>
       <c r="B6" s="1">
-        <v>1399.8589999999999</v>
+        <v>1381.9870000000001</v>
       </c>
       <c r="C6" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D6" s="1">
-        <v>-7.95</v>
+        <v>-7.92</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>865.15499999999997</v>
+        <v>901.06899999999996</v>
       </c>
       <c r="B7" s="1">
-        <v>1305.21</v>
+        <v>1289.6510000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D7" s="1">
-        <v>-5.98</v>
+        <v>-5.9</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>863.11300000000006</v>
+        <v>899.51700000000005</v>
       </c>
       <c r="B8" s="1">
-        <v>1210.49</v>
+        <v>1198.7180000000001</v>
       </c>
       <c r="C8" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D8" s="1">
-        <v>-3.98</v>
+        <v>-3.9</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>861.14700000000005</v>
+        <v>898.83600000000001</v>
       </c>
       <c r="B9" s="1">
-        <v>1115.7159999999999</v>
+        <v>1107.4749999999999</v>
       </c>
       <c r="C9" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D9" s="1">
-        <v>-1.98</v>
+        <v>-1.9</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>860.23800000000006</v>
+        <v>898.52200000000005</v>
       </c>
       <c r="B10" s="1">
-        <v>1021.248</v>
+        <v>1017.811</v>
       </c>
       <c r="C10" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>859.56399999999996</v>
+        <v>899.00699999999995</v>
       </c>
       <c r="B11" s="1">
-        <v>925.76900000000001</v>
+        <v>927.048</v>
       </c>
       <c r="C11" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D11" s="1">
-        <v>2</v>
+        <v>2.08</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>859.44299999999998</v>
+        <v>899.92399999999998</v>
       </c>
       <c r="B12" s="1">
-        <v>829.29</v>
+        <v>836.10599999999999</v>
       </c>
       <c r="C12" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D12" s="1">
-        <v>4</v>
+        <v>4.08</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>860.28499999999997</v>
+        <v>901.47799999999995</v>
       </c>
       <c r="B13" s="1">
-        <v>732.84299999999996</v>
+        <v>745.47799999999995</v>
       </c>
       <c r="C13" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D13" s="1">
-        <v>5.97</v>
+        <v>6.08</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>861.23400000000004</v>
+        <v>903.56200000000001</v>
       </c>
       <c r="B14" s="1">
-        <v>633.27</v>
+        <v>653.49099999999999</v>
       </c>
       <c r="C14" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D14" s="1">
-        <v>7.9</v>
+        <v>8.08</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>863.35400000000004</v>
+        <v>906.39599999999996</v>
       </c>
       <c r="B15" s="1">
-        <v>530.68200000000002</v>
+        <v>560.06100000000004</v>
       </c>
       <c r="C15" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D15" s="1">
-        <v>10.029999999999999</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>865.52300000000002</v>
+        <v>910.07799999999997</v>
       </c>
       <c r="B16" s="1">
-        <v>432.35199999999998</v>
+        <v>462.47800000000001</v>
       </c>
       <c r="C16" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D16" s="1">
-        <v>11.98</v>
+        <v>12.07</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>868.69399999999996</v>
+        <v>914.46699999999998</v>
       </c>
       <c r="B17" s="1">
-        <v>331.108</v>
+        <v>367.52300000000002</v>
       </c>
       <c r="C17" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D17" s="1">
-        <v>13.98</v>
+        <v>14.07</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>872.149</v>
+        <v>918.90300000000002</v>
       </c>
       <c r="B18" s="1">
-        <v>227.54300000000001</v>
+        <v>271.791</v>
       </c>
       <c r="C18" s="1">
-        <v>2502.6999999999998</v>
+        <v>2501.4</v>
       </c>
       <c r="D18" s="1">
-        <v>15.98</v>
+        <v>16.07</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>841.39800000000002</v>
+        <v>879.70600000000002</v>
       </c>
       <c r="B19" s="1">
-        <v>1022.364</v>
+        <v>1022.107</v>
       </c>
       <c r="C19" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -637,268 +637,268 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>865.41099999999994</v>
+        <v>898.36900000000003</v>
       </c>
       <c r="B20" s="1">
-        <v>1796.1479999999999</v>
+        <v>1773.366</v>
       </c>
       <c r="C20" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D20" s="1">
-        <v>-16.07</v>
+        <v>-16.079999999999998</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>860.15300000000002</v>
+        <v>893.55</v>
       </c>
       <c r="B21" s="1">
-        <v>1691.172</v>
+        <v>1669.5709999999999</v>
       </c>
       <c r="C21" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D21" s="1">
-        <v>-13.98</v>
+        <v>-14</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>855.74900000000002</v>
+        <v>889.76099999999997</v>
       </c>
       <c r="B22" s="1">
-        <v>1592.172</v>
+        <v>1570.2</v>
       </c>
       <c r="C22" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D22" s="1">
-        <v>-11.98</v>
+        <v>-11.92</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>851.89599999999996</v>
+        <v>886.53700000000003</v>
       </c>
       <c r="B23" s="1">
-        <v>1495.318</v>
+        <v>1475.625</v>
       </c>
       <c r="C23" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D23" s="1">
-        <v>-9.98</v>
+        <v>-9.9499999999999993</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>848.86599999999999</v>
+        <v>883.91</v>
       </c>
       <c r="B24" s="1">
-        <v>1399.1569999999999</v>
+        <v>1381.73</v>
       </c>
       <c r="C24" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D24" s="1">
-        <v>-7.95</v>
+        <v>-7.92</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>846.35699999999997</v>
+        <v>882.149</v>
       </c>
       <c r="B25" s="1">
-        <v>1304.6030000000001</v>
+        <v>1288.855</v>
       </c>
       <c r="C25" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D25" s="1">
-        <v>-5.98</v>
+        <v>-5.92</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>844.221</v>
+        <v>880.721</v>
       </c>
       <c r="B26" s="1">
-        <v>1209.913</v>
+        <v>1197.213</v>
       </c>
       <c r="C26" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D26" s="1">
-        <v>-3.98</v>
+        <v>-3.9</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>842.48400000000004</v>
+        <v>879.98199999999997</v>
       </c>
       <c r="B27" s="1">
-        <v>1114.93</v>
+        <v>1107.701</v>
       </c>
       <c r="C27" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D27" s="1">
-        <v>-1.98</v>
+        <v>-1.9</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>841.39599999999996</v>
+        <v>879.75900000000001</v>
       </c>
       <c r="B28" s="1">
-        <v>1021.222</v>
+        <v>1016.862</v>
       </c>
       <c r="C28" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>840.85599999999999</v>
+        <v>880.07100000000003</v>
       </c>
       <c r="B29" s="1">
-        <v>925.36500000000001</v>
+        <v>927.42100000000005</v>
       </c>
       <c r="C29" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D29" s="1">
-        <v>2</v>
+        <v>2.08</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>840.50800000000004</v>
+        <v>880.98</v>
       </c>
       <c r="B30" s="1">
-        <v>829.30799999999999</v>
+        <v>836.30100000000004</v>
       </c>
       <c r="C30" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D30" s="1">
-        <v>4</v>
+        <v>4.08</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>841.28099999999995</v>
+        <v>882.52</v>
       </c>
       <c r="B31" s="1">
-        <v>733.95</v>
+        <v>744.53099999999995</v>
       </c>
       <c r="C31" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D31" s="1">
-        <v>5.97</v>
+        <v>6.08</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>842.09400000000005</v>
+        <v>884.51599999999996</v>
       </c>
       <c r="B32" s="1">
-        <v>633.88900000000001</v>
+        <v>652.64499999999998</v>
       </c>
       <c r="C32" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D32" s="1">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>844.3</v>
+        <v>887.19899999999996</v>
       </c>
       <c r="B33" s="1">
-        <v>531.29300000000001</v>
+        <v>560.41600000000005</v>
       </c>
       <c r="C33" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D33" s="1">
-        <v>10.029999999999999</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>846.43499999999995</v>
+        <v>890.94299999999998</v>
       </c>
       <c r="B34" s="1">
-        <v>432.97300000000001</v>
+        <v>463.13299999999998</v>
       </c>
       <c r="C34" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D34" s="1">
-        <v>11.98</v>
+        <v>12.07</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>849.16700000000003</v>
+        <v>895.03899999999999</v>
       </c>
       <c r="B35" s="1">
-        <v>331.608</v>
+        <v>368.02</v>
       </c>
       <c r="C35" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D35" s="1">
-        <v>13.98</v>
+        <v>14.07</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>852.86900000000003</v>
+        <v>899.24099999999999</v>
       </c>
       <c r="B36" s="1">
-        <v>228.44800000000001</v>
+        <v>272.52999999999997</v>
       </c>
       <c r="C36" s="1">
-        <v>2602.4</v>
+        <v>2601.1</v>
       </c>
       <c r="D36" s="1">
-        <v>15.98</v>
+        <v>16.07</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>823.84</v>
+        <v>862.15899999999999</v>
       </c>
       <c r="B37" s="1">
-        <v>1022.085</v>
+        <v>1022.354</v>
       </c>
       <c r="C37" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -907,28 +907,28 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>847.88400000000001</v>
+        <v>880.36400000000003</v>
       </c>
       <c r="B38" s="1">
-        <v>1795.79</v>
+        <v>1773.1179999999999</v>
       </c>
       <c r="C38" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D38" s="1">
-        <v>-16.07</v>
+        <v>-16.079999999999998</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>842.41700000000003</v>
+        <v>875.57500000000005</v>
       </c>
       <c r="B39" s="1">
-        <v>1690.653</v>
+        <v>1669.5440000000001</v>
       </c>
       <c r="C39" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D39" s="1">
         <v>-14</v>
@@ -937,28 +937,28 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>838.23299999999995</v>
+        <v>871.79899999999998</v>
       </c>
       <c r="B40" s="1">
-        <v>1590.575</v>
+        <v>1570.374</v>
       </c>
       <c r="C40" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D40" s="1">
-        <v>-11.98</v>
+        <v>-11.92</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>834.33299999999997</v>
+        <v>868.79200000000003</v>
       </c>
       <c r="B41" s="1">
-        <v>1493.7729999999999</v>
+        <v>1475.4359999999999</v>
       </c>
       <c r="C41" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D41" s="1">
         <v>-9.9499999999999993</v>
@@ -967,208 +967,208 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>831.37599999999998</v>
+        <v>866.41600000000005</v>
       </c>
       <c r="B42" s="1">
-        <v>1398.8030000000001</v>
+        <v>1381.414</v>
       </c>
       <c r="C42" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D42" s="1">
-        <v>-7.95</v>
+        <v>-7.92</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>829</v>
+        <v>864.51199999999994</v>
       </c>
       <c r="B43" s="1">
-        <v>1304.953</v>
+        <v>1288.751</v>
       </c>
       <c r="C43" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D43" s="1">
-        <v>-5.98</v>
+        <v>-5.92</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>826.78200000000004</v>
+        <v>863.08299999999997</v>
       </c>
       <c r="B44" s="1">
-        <v>1209.893</v>
+        <v>1197.0029999999999</v>
       </c>
       <c r="C44" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D44" s="1">
-        <v>-4</v>
+        <v>-3.9</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>825.05200000000002</v>
+        <v>862.35799999999995</v>
       </c>
       <c r="B45" s="1">
-        <v>1114.356</v>
+        <v>1107.9970000000001</v>
       </c>
       <c r="C45" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D45" s="1">
-        <v>-1.98</v>
+        <v>-1.9</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>823.85699999999997</v>
+        <v>862.12300000000005</v>
       </c>
       <c r="B46" s="1">
-        <v>1019.814</v>
+        <v>1017.1420000000001</v>
       </c>
       <c r="C46" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D46" s="1">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>823.20500000000004</v>
+        <v>862.69200000000001</v>
       </c>
       <c r="B47" s="1">
-        <v>926.25199999999995</v>
+        <v>928.47199999999998</v>
       </c>
       <c r="C47" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D47" s="1">
-        <v>2</v>
+        <v>2.08</v>
       </c>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>823.31399999999996</v>
+        <v>863.55700000000002</v>
       </c>
       <c r="B48" s="1">
-        <v>830.37599999999998</v>
+        <v>837.05799999999999</v>
       </c>
       <c r="C48" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D48" s="1">
-        <v>3.98</v>
+        <v>4.08</v>
       </c>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>823.75199999999995</v>
+        <v>864.99300000000005</v>
       </c>
       <c r="B49" s="1">
-        <v>732.17499999999995</v>
+        <v>745.12099999999998</v>
       </c>
       <c r="C49" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D49" s="1">
-        <v>6</v>
+        <v>6.08</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>824.89200000000005</v>
+        <v>867.03499999999997</v>
       </c>
       <c r="B50" s="1">
-        <v>634.31399999999996</v>
+        <v>653.64400000000001</v>
       </c>
       <c r="C50" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D50" s="1">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>826.5</v>
+        <v>869.50099999999998</v>
       </c>
       <c r="B51" s="1">
-        <v>531.81799999999998</v>
+        <v>562.05700000000002</v>
       </c>
       <c r="C51" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D51" s="1">
-        <v>10.029999999999999</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>828.50599999999997</v>
+        <v>873.029</v>
       </c>
       <c r="B52" s="1">
-        <v>434.83800000000002</v>
+        <v>464.23099999999999</v>
       </c>
       <c r="C52" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D52" s="1">
-        <v>11.98</v>
+        <v>12.07</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>831.02099999999996</v>
+        <v>876.96400000000006</v>
       </c>
       <c r="B53" s="1">
-        <v>333.15699999999998</v>
+        <v>369.44200000000001</v>
       </c>
       <c r="C53" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D53" s="1">
-        <v>13.98</v>
+        <v>14.07</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>834.72400000000005</v>
+        <v>881.15599999999995</v>
       </c>
       <c r="B54" s="1">
-        <v>228.64699999999999</v>
+        <v>273.88299999999998</v>
       </c>
       <c r="C54" s="1">
-        <v>2702.1</v>
+        <v>2700.8</v>
       </c>
       <c r="D54" s="1">
-        <v>16</v>
+        <v>16.07</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>807.90800000000002</v>
+        <v>846</v>
       </c>
       <c r="B55" s="1">
-        <v>1022.21</v>
+        <v>1022.515</v>
       </c>
       <c r="C55" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -1177,43 +1177,43 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>831.14200000000005</v>
+        <v>863.48299999999995</v>
       </c>
       <c r="B56" s="1">
-        <v>1794.463</v>
+        <v>1772.249</v>
       </c>
       <c r="C56" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D56" s="1">
-        <v>-16.07</v>
+        <v>-16.079999999999998</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>825.97500000000002</v>
+        <v>859.01499999999999</v>
       </c>
       <c r="B57" s="1">
-        <v>1689.8710000000001</v>
+        <v>1668.0989999999999</v>
       </c>
       <c r="C57" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D57" s="1">
-        <v>-14</v>
+        <v>-13.97</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>821.96699999999998</v>
+        <v>855.5</v>
       </c>
       <c r="B58" s="1">
-        <v>1590.06</v>
+        <v>1570.4839999999999</v>
       </c>
       <c r="C58" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D58" s="1">
         <v>-11.95</v>
@@ -1222,223 +1222,223 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>818.17399999999998</v>
+        <v>852.495</v>
       </c>
       <c r="B59" s="1">
-        <v>1494.5920000000001</v>
+        <v>1475.377</v>
       </c>
       <c r="C59" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D59" s="1">
-        <v>-9.98</v>
+        <v>-9.9499999999999993</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>815.18899999999996</v>
+        <v>850.197</v>
       </c>
       <c r="B60" s="1">
-        <v>1397.7439999999999</v>
+        <v>1381.1</v>
       </c>
       <c r="C60" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D60" s="1">
-        <v>-7.95</v>
+        <v>-7.92</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>812.654</v>
+        <v>848.19600000000003</v>
       </c>
       <c r="B61" s="1">
-        <v>1304.1489999999999</v>
+        <v>1288.557</v>
       </c>
       <c r="C61" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D61" s="1">
-        <v>-5.98</v>
+        <v>-5.9</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>810.60900000000004</v>
+        <v>846.99599999999998</v>
       </c>
       <c r="B62" s="1">
-        <v>1209.675</v>
+        <v>1198.04</v>
       </c>
       <c r="C62" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D62" s="1">
-        <v>-3.98</v>
+        <v>-3.92</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>808.87199999999996</v>
+        <v>846.19200000000001</v>
       </c>
       <c r="B63" s="1">
-        <v>1115.06</v>
+        <v>1107.692</v>
       </c>
       <c r="C63" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D63" s="1">
-        <v>-2</v>
+        <v>-1.9</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>807.80899999999997</v>
+        <v>846.00800000000004</v>
       </c>
       <c r="B64" s="1">
-        <v>1019.702</v>
+        <v>1017.655</v>
       </c>
       <c r="C64" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D64" s="1">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>807.09299999999996</v>
+        <v>846.32</v>
       </c>
       <c r="B65" s="1">
-        <v>926.10500000000002</v>
+        <v>928.36599999999999</v>
       </c>
       <c r="C65" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D65" s="1">
-        <v>2</v>
+        <v>2.08</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>807.15800000000002</v>
+        <v>847.16899999999998</v>
       </c>
       <c r="B66" s="1">
-        <v>829.67100000000005</v>
+        <v>837.75400000000002</v>
       </c>
       <c r="C66" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D66" s="1">
-        <v>3.98</v>
+        <v>4.08</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>807.53700000000003</v>
+        <v>848.69</v>
       </c>
       <c r="B67" s="1">
-        <v>732.92399999999998</v>
+        <v>745.70899999999995</v>
       </c>
       <c r="C67" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D67" s="1">
-        <v>6</v>
+        <v>6.08</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>808.43299999999999</v>
+        <v>850.59900000000005</v>
       </c>
       <c r="B68" s="1">
-        <v>635.31299999999999</v>
+        <v>653.87300000000005</v>
       </c>
       <c r="C68" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D68" s="1">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>810.17600000000004</v>
+        <v>853.29499999999996</v>
       </c>
       <c r="B69" s="1">
-        <v>532.30499999999995</v>
+        <v>563.17499999999995</v>
       </c>
       <c r="C69" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D69" s="1">
-        <v>10.029999999999999</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>811.96500000000003</v>
+        <v>856.45500000000004</v>
       </c>
       <c r="B70" s="1">
-        <v>435.18799999999999</v>
+        <v>465.673</v>
       </c>
       <c r="C70" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D70" s="1">
-        <v>11.98</v>
+        <v>12.07</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>814.78499999999997</v>
+        <v>860.36800000000005</v>
       </c>
       <c r="B71" s="1">
-        <v>334.28100000000001</v>
+        <v>370.78199999999998</v>
       </c>
       <c r="C71" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D71" s="1">
-        <v>13.98</v>
+        <v>14.07</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>817.87599999999998</v>
+        <v>864.45299999999997</v>
       </c>
       <c r="B72" s="1">
-        <v>231.21899999999999</v>
+        <v>275.21699999999998</v>
       </c>
       <c r="C72" s="1">
-        <v>2801.8</v>
+        <v>2800.5</v>
       </c>
       <c r="D72" s="1">
-        <v>15.98</v>
+        <v>16.07</v>
       </c>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>792.95100000000002</v>
+        <v>831.053</v>
       </c>
       <c r="B73" s="1">
-        <v>1022.16</v>
+        <v>1022.304</v>
       </c>
       <c r="C73" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -1447,43 +1447,43 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>815.94100000000003</v>
+        <v>847.99699999999996</v>
       </c>
       <c r="B74" s="1">
-        <v>1793.693</v>
+        <v>1772.45</v>
       </c>
       <c r="C74" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D74" s="1">
-        <v>-16.07</v>
+        <v>-16.079999999999998</v>
       </c>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>810.86800000000005</v>
+        <v>843.52200000000005</v>
       </c>
       <c r="B75" s="1">
-        <v>1689.1179999999999</v>
+        <v>1668.181</v>
       </c>
       <c r="C75" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D75" s="1">
-        <v>-14</v>
+        <v>-13.97</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>806.64200000000005</v>
+        <v>840.33</v>
       </c>
       <c r="B76" s="1">
-        <v>1589.5360000000001</v>
+        <v>1570.356</v>
       </c>
       <c r="C76" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D76" s="1">
         <v>-11.95</v>
@@ -1492,223 +1492,223 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>803.21600000000001</v>
+        <v>837.44</v>
       </c>
       <c r="B77" s="1">
-        <v>1493.8109999999999</v>
+        <v>1475.73</v>
       </c>
       <c r="C77" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D77" s="1">
-        <v>-9.98</v>
+        <v>-9.9499999999999993</v>
       </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>800.25900000000001</v>
+        <v>834.95399999999995</v>
       </c>
       <c r="B78" s="1">
-        <v>1397.625</v>
+        <v>1381.511</v>
       </c>
       <c r="C78" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D78" s="1">
-        <v>-7.95</v>
+        <v>-7.92</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>797.69399999999996</v>
+        <v>833.19799999999998</v>
       </c>
       <c r="B79" s="1">
-        <v>1303.8720000000001</v>
+        <v>1288.9760000000001</v>
       </c>
       <c r="C79" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D79" s="1">
-        <v>-5.98</v>
+        <v>-5.9</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>795.57500000000005</v>
+        <v>831.995</v>
       </c>
       <c r="B80" s="1">
-        <v>1209.395</v>
+        <v>1198.3889999999999</v>
       </c>
       <c r="C80" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D80" s="1">
-        <v>-3.98</v>
+        <v>-3.92</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>793.84500000000003</v>
+        <v>831.24</v>
       </c>
       <c r="B81" s="1">
-        <v>1114.6079999999999</v>
+        <v>1108.5999999999999</v>
       </c>
       <c r="C81" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D81" s="1">
-        <v>-2</v>
+        <v>-1.9</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>792.93299999999999</v>
+        <v>831.048</v>
       </c>
       <c r="B82" s="1">
-        <v>1019.715</v>
+        <v>1018.276</v>
       </c>
       <c r="C82" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D82" s="1">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>792.16600000000005</v>
+        <v>831.29200000000003</v>
       </c>
       <c r="B83" s="1">
-        <v>926.12599999999998</v>
+        <v>929.05200000000002</v>
       </c>
       <c r="C83" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D83" s="1">
-        <v>2</v>
+        <v>2.08</v>
       </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>791.87800000000004</v>
+        <v>832.16700000000003</v>
       </c>
       <c r="B84" s="1">
-        <v>829.96600000000001</v>
+        <v>838.23199999999997</v>
       </c>
       <c r="C84" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D84" s="1">
-        <v>3.98</v>
+        <v>4.08</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>792.42200000000003</v>
+        <v>833.72500000000002</v>
       </c>
       <c r="B85" s="1">
-        <v>732.70600000000002</v>
+        <v>747.28599999999994</v>
       </c>
       <c r="C85" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D85" s="1">
-        <v>6</v>
+        <v>6.08</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>793.30399999999997</v>
+        <v>835.51599999999996</v>
       </c>
       <c r="B86" s="1">
-        <v>635.48900000000003</v>
+        <v>655.32399999999996</v>
       </c>
       <c r="C86" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D86" s="1">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>794.62400000000002</v>
+        <v>837.77</v>
       </c>
       <c r="B87" s="1">
-        <v>534.053</v>
+        <v>564.03300000000002</v>
       </c>
       <c r="C87" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D87" s="1">
-        <v>10.029999999999999</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>796.60900000000004</v>
+        <v>841.07899999999995</v>
       </c>
       <c r="B88" s="1">
-        <v>436.17099999999999</v>
+        <v>466.315</v>
       </c>
       <c r="C88" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D88" s="1">
-        <v>11.98</v>
+        <v>12.07</v>
       </c>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>799.04</v>
+        <v>844.92700000000002</v>
       </c>
       <c r="B89" s="1">
-        <v>334.43900000000002</v>
+        <v>371.988</v>
       </c>
       <c r="C89" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D89" s="1">
-        <v>13.98</v>
+        <v>14.07</v>
       </c>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>802.14</v>
+        <v>848.98</v>
       </c>
       <c r="B90" s="1">
-        <v>231.17</v>
+        <v>275.97399999999999</v>
       </c>
       <c r="C90" s="1">
-        <v>2901.5</v>
+        <v>2900.2</v>
       </c>
       <c r="D90" s="1">
-        <v>15.98</v>
+        <v>16.07</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
-        <v>778.90499999999997</v>
+        <v>816.94799999999998</v>
       </c>
       <c r="B91" s="1">
-        <v>1022.193</v>
+        <v>1022.534</v>
       </c>
       <c r="C91" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -1717,13 +1717,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
-        <v>801.58100000000002</v>
+        <v>833.42</v>
       </c>
       <c r="B92" s="1">
-        <v>1792.097</v>
+        <v>1770.712</v>
       </c>
       <c r="C92" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D92" s="1">
         <v>-16.07</v>
@@ -1732,13 +1732,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
-        <v>796.13199999999995</v>
+        <v>829.38099999999997</v>
       </c>
       <c r="B93" s="1">
-        <v>1687.26</v>
+        <v>1666.7629999999999</v>
       </c>
       <c r="C93" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D93" s="1">
         <v>-13.98</v>
@@ -1747,43 +1747,43 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
-        <v>792.52800000000002</v>
+        <v>825.851</v>
       </c>
       <c r="B94" s="1">
-        <v>1590.105</v>
+        <v>1569.5509999999999</v>
       </c>
       <c r="C94" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D94" s="1">
-        <v>-11.98</v>
+        <v>-11.95</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
-        <v>789.04</v>
+        <v>823.26800000000003</v>
       </c>
       <c r="B95" s="1">
-        <v>1492.422</v>
+        <v>1474.0239999999999</v>
       </c>
       <c r="C95" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D95" s="1">
-        <v>-9.98</v>
+        <v>-9.93</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
-        <v>786.17200000000003</v>
+        <v>820.87900000000002</v>
       </c>
       <c r="B96" s="1">
-        <v>1397.395</v>
+        <v>1381.4849999999999</v>
       </c>
       <c r="C96" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D96" s="1">
         <v>-7.95</v>
@@ -1792,181 +1792,181 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
-        <v>783.60699999999997</v>
+        <v>819.12199999999996</v>
       </c>
       <c r="B97" s="1">
-        <v>1303.8309999999999</v>
+        <v>1287.595</v>
       </c>
       <c r="C97" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D97" s="1">
-        <v>-5.98</v>
+        <v>-5.9</v>
       </c>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
-        <v>781.51</v>
+        <v>817.98199999999997</v>
       </c>
       <c r="B98" s="1">
-        <v>1209.0550000000001</v>
+        <v>1197.1769999999999</v>
       </c>
       <c r="C98" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D98" s="1">
-        <v>-3.98</v>
+        <v>-3.93</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
-        <v>779.84799999999996</v>
+        <v>817.14800000000002</v>
       </c>
       <c r="B99" s="1">
-        <v>1114.96</v>
+        <v>1107.702</v>
       </c>
       <c r="C99" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D99" s="1">
-        <v>-1.98</v>
+        <v>-1.9</v>
       </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
-        <v>778.89499999999998</v>
+        <v>816.96</v>
       </c>
       <c r="B100" s="1">
-        <v>1020.748</v>
+        <v>1017.477</v>
       </c>
       <c r="C100" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D100" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
-        <v>778.21400000000006</v>
+        <v>817.37199999999996</v>
       </c>
       <c r="B101" s="1">
-        <v>926.072</v>
+        <v>926.98599999999999</v>
       </c>
       <c r="C101" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D101" s="1">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
-        <v>777.92600000000004</v>
+        <v>818.096</v>
       </c>
       <c r="B102" s="1">
-        <v>830.11099999999999</v>
+        <v>837.17700000000002</v>
       </c>
       <c r="C102" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D102" s="1">
-        <v>4</v>
+        <v>4.08</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
-        <v>778.17</v>
+        <v>819.70799999999997</v>
       </c>
       <c r="B103" s="1">
-        <v>734.48099999999999</v>
+        <v>746.33199999999999</v>
       </c>
       <c r="C103" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D103" s="1">
-        <v>5.97</v>
+        <v>6.08</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
-        <v>779.322</v>
+        <v>821.48</v>
       </c>
       <c r="B104" s="1">
-        <v>635.94500000000005</v>
+        <v>654.48500000000001</v>
       </c>
       <c r="C104" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D104" s="1">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
-        <v>780.53899999999999</v>
+        <v>823.56</v>
       </c>
       <c r="B105" s="1">
-        <v>534.26900000000001</v>
+        <v>563.62400000000002</v>
       </c>
       <c r="C105" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D105" s="1">
-        <v>10.029999999999999</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
-        <v>782.20799999999997</v>
+        <v>826.99400000000003</v>
       </c>
       <c r="B106" s="1">
-        <v>436.76100000000002</v>
+        <v>464.58600000000001</v>
       </c>
       <c r="C106" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D106" s="1">
-        <v>11.98</v>
+        <v>12.1</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>784.86400000000003</v>
+        <v>830.745</v>
       </c>
       <c r="B107" s="1">
-        <v>334.97899999999998</v>
+        <v>370.28</v>
       </c>
       <c r="C107" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D107" s="1">
-        <v>13.98</v>
+        <v>14.1</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>787.54300000000001</v>
+        <v>834.31200000000001</v>
       </c>
       <c r="B108" s="1">
-        <v>232.44</v>
+        <v>275.64100000000002</v>
       </c>
       <c r="C108" s="1">
-        <v>3001.1</v>
+        <v>2999.8</v>
       </c>
       <c r="D108" s="1">
-        <v>15.98</v>
+        <v>16.07</v>
       </c>
       <c r="E108" s="1"/>
     </row>

</xml_diff>